<commit_message>
Finished gathering data for sobel classification in excel. Attached excel and some photos of predicted masks
</commit_message>
<xml_diff>
--- a/MicroPasts_documents/LinearSVC_table.xlsx
+++ b/MicroPasts_documents/LinearSVC_table.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="18">
   <si>
     <t>Object</t>
   </si>
@@ -51,17 +52,32 @@
     <t>DecisionTree</t>
   </si>
   <si>
-    <t>Downsampling</t>
+    <t>Layers of Sobel</t>
   </si>
   <si>
-    <t>Blur per sobel layer</t>
+    <t>RGB included</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>IMPORTANT NOTE: The Errors on this page are 16 times smaller than RGB_Feature because the images are rescaled by 0.25 at the start</t>
+  </si>
+  <si>
+    <t>Normalised Test Er</t>
+  </si>
+  <si>
+    <t>Normalised Train Er</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,13 +85,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -90,10 +139,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,7 +449,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I2"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -957,22 +1015,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="11" max="11" width="11" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1003,8 +1063,14 @@
       <c r="J1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1015,28 +1081,39 @@
         <v>100</v>
       </c>
       <c r="D2" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="2">
-        <v>711772</v>
+        <v>62800</v>
       </c>
       <c r="G2" s="2">
-        <v>930766</v>
+        <v>110000</v>
       </c>
       <c r="H2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>10</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2">
+        <f>F2*M2</f>
+        <v>1004800</v>
+      </c>
+      <c r="L2" s="2">
+        <f>G2*M2</f>
+        <v>1760000</v>
+      </c>
+      <c r="M2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1047,29 +1124,984 @@
         <v>100</v>
       </c>
       <c r="D3" s="1">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2">
+        <v>72000</v>
+      </c>
+      <c r="G3" s="2">
+        <v>85000</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>9</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="2">
+        <f>F3*M3</f>
+        <v>1152000</v>
+      </c>
+      <c r="L3" s="2">
+        <f t="shared" ref="L3:L16" si="0">G3*M3</f>
+        <v>1360000</v>
+      </c>
+      <c r="M3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4" s="1">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2">
+        <v>138000</v>
+      </c>
+      <c r="G4" s="2">
+        <v>155000</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2">
-        <v>864778</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1161111</v>
-      </c>
-      <c r="H3">
-        <v>6</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
+      <c r="J4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" ref="K4:K16" si="1">F4*M4</f>
+        <v>2208000</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" si="0"/>
+        <v>2480000</v>
+      </c>
+      <c r="M4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5" s="1">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2">
+        <v>158000</v>
+      </c>
+      <c r="G5" s="2">
+        <v>196000</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>7</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="1"/>
+        <v>2528000</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" si="0"/>
+        <v>3136000</v>
+      </c>
+      <c r="M5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6" s="1">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2">
+        <v>168000</v>
+      </c>
+      <c r="G6" s="2">
+        <v>180000</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="1"/>
+        <v>2688000</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" si="0"/>
+        <v>2880000</v>
+      </c>
+      <c r="M6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7" s="1">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2">
+        <v>172000</v>
+      </c>
+      <c r="G7" s="2">
+        <v>170000</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="1"/>
+        <v>2752000</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="0"/>
+        <v>2720000</v>
+      </c>
+      <c r="M7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8" s="1">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="2">
+        <v>185000</v>
+      </c>
+      <c r="G8" s="2">
+        <v>210000</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="1"/>
+        <v>2960000</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="0"/>
+        <v>3360000</v>
+      </c>
+      <c r="M8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9" s="1">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="2">
+        <v>185000</v>
+      </c>
+      <c r="G9" s="2">
+        <v>180000</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="1"/>
+        <v>2960000</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="0"/>
+        <v>2880000</v>
+      </c>
+      <c r="M9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10" s="1">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="2">
+        <v>204000</v>
+      </c>
+      <c r="G10" s="2">
+        <v>200000</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="1"/>
+        <v>3264000</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="0"/>
+        <v>3200000</v>
+      </c>
+      <c r="M10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11" s="1">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="2">
+        <v>189000</v>
+      </c>
+      <c r="G11" s="2">
+        <v>185000</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
         <v>1</v>
       </c>
+      <c r="J11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="1"/>
+        <v>3024000</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="0"/>
+        <v>2960000</v>
+      </c>
+      <c r="M11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+      <c r="D12" s="1">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="2">
+        <v>76000</v>
+      </c>
+      <c r="G12" s="2">
+        <v>85000</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="1"/>
+        <v>1216000</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="0"/>
+        <v>1360000</v>
+      </c>
+      <c r="M12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>100</v>
+      </c>
+      <c r="D13" s="1">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="2">
+        <v>49000</v>
+      </c>
+      <c r="G13" s="2">
+        <v>54000</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>5</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="1"/>
+        <v>784000</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="0"/>
+        <v>864000</v>
+      </c>
+      <c r="M13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14" s="1">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="2">
+        <v>43500</v>
+      </c>
+      <c r="G14" s="2">
+        <v>80000</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>9</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="1"/>
+        <v>696000</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="0"/>
+        <v>1280000</v>
+      </c>
+      <c r="M14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="10">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>100</v>
+      </c>
+      <c r="D15" s="1">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="2">
+        <v>37700</v>
+      </c>
+      <c r="G15" s="2">
+        <v>45000</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>9</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="1"/>
+        <v>603200</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="0"/>
+        <v>720000</v>
+      </c>
+      <c r="M15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>100</v>
+      </c>
+      <c r="D16" s="1">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="2">
+        <v>52600</v>
+      </c>
+      <c r="G16" s="2">
+        <v>65000</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+      <c r="I16">
+        <v>10</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="1"/>
+        <v>841600</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="0"/>
+        <v>1040000</v>
+      </c>
+      <c r="M16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" s="10">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="2">
+        <v>169000</v>
+      </c>
+      <c r="G17" s="2">
+        <v>170000</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" ref="K17:K19" si="2">F17*M17</f>
+        <v>2704000</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" ref="L17:L19" si="3">G17*M17</f>
+        <v>2720000</v>
+      </c>
+      <c r="M17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" s="10">
+        <v>1000</v>
+      </c>
+      <c r="D18" s="1">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="2">
+        <v>27000</v>
+      </c>
+      <c r="G18" s="2">
+        <v>35000</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" si="2"/>
+        <v>432000</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="3"/>
+        <v>560000</v>
+      </c>
+      <c r="M18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19" s="10">
+        <v>10000</v>
+      </c>
+      <c r="D19" s="1">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="2">
+        <v>9968</v>
+      </c>
+      <c r="G19" s="2">
+        <v>17000</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" si="2"/>
+        <v>159488</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="3"/>
+        <v>272000</v>
+      </c>
+      <c r="M19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20" s="10">
+        <v>100000</v>
+      </c>
+      <c r="D20" s="1">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="2">
+        <v>3110</v>
+      </c>
+      <c r="G20" s="2">
+        <v>17000</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20">
+        <v>5</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" ref="K20:K26" si="4">F20*M20</f>
+        <v>49760</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" ref="L20:L26" si="5">G20*M20</f>
+        <v>272000</v>
+      </c>
+      <c r="M20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" s="5">
+        <v>10000</v>
+      </c>
+      <c r="D21" s="11">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="2">
+        <v>10200</v>
+      </c>
+      <c r="G21" s="2">
+        <v>15500</v>
+      </c>
+      <c r="H21" s="10">
+        <v>6</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="4"/>
+        <v>163200</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="5"/>
+        <v>248000</v>
+      </c>
+      <c r="M21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5">
+        <v>10000</v>
+      </c>
+      <c r="D22" s="1">
+        <v>16</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="2">
+        <v>2340</v>
+      </c>
+      <c r="G22" s="2">
+        <v>30000</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22" s="10">
+        <v>9</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="4"/>
+        <v>37440</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="5"/>
+        <v>480000</v>
+      </c>
+      <c r="M22">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="10">
+        <v>1</v>
+      </c>
+      <c r="C23" s="5">
+        <v>10000</v>
+      </c>
+      <c r="D23" s="1">
+        <v>16</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="2">
+        <v>4500</v>
+      </c>
+      <c r="G23" s="2">
+        <v>27000</v>
+      </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+      <c r="I23" s="5">
+        <v>9</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" ref="K23:K26" si="6">F23*M23</f>
+        <v>72000</v>
+      </c>
+      <c r="L23" s="2">
+        <f t="shared" ref="L23:L26" si="7">G23*M23</f>
+        <v>432000</v>
+      </c>
+      <c r="M23">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24" s="5">
+        <v>10000</v>
+      </c>
+      <c r="D24" s="1">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="2">
+        <v>7500</v>
+      </c>
+      <c r="G24" s="2">
+        <v>20000</v>
+      </c>
+      <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="I24" s="5">
+        <v>7</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="6"/>
+        <v>120000</v>
+      </c>
+      <c r="L24" s="2">
+        <f t="shared" si="7"/>
+        <v>320000</v>
+      </c>
+      <c r="M24">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="C25" s="5"/>
+      <c r="D25" s="1"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="C26" s="5"/>
+      <c r="D26" s="1"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="C27" s="5"/>
+      <c r="D27" s="1"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="C28" s="5"/>
+      <c r="D28" s="1"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Uploading watershed scripts for first time
Also modified useClassifier to create a file and fill with predicted
masks (currently using superpixels)
</commit_message>
<xml_diff>
--- a/MicroPasts_documents/LinearSVC_table.xlsx
+++ b/MicroPasts_documents/LinearSVC_table.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="19">
   <si>
     <t>Object</t>
   </si>
@@ -72,11 +71,17 @@
   <si>
     <t>Normalised Train Er</t>
   </si>
+  <si>
+    <t>% error</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -139,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -152,6 +157,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,7 +455,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1015,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1029,10 +1035,11 @@
     <col min="7" max="7" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="11" max="11" width="11" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1069,8 +1076,11 @@
       <c r="L1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="M1" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1102,18 +1112,22 @@
         <v>14</v>
       </c>
       <c r="K2" s="2">
-        <f>F2*M2</f>
+        <f>F2*N2</f>
         <v>1004800</v>
       </c>
       <c r="L2" s="2">
-        <f>G2*M2</f>
+        <f>G2*N2</f>
         <v>1760000</v>
       </c>
-      <c r="M2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="M2" s="12">
+        <f>L2/(17900000)</f>
+        <v>9.8324022346368709E-2</v>
+      </c>
+      <c r="N2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1145,18 +1159,22 @@
         <v>14</v>
       </c>
       <c r="K3" s="2">
-        <f>F3*M3</f>
+        <f>F3*N3</f>
         <v>1152000</v>
       </c>
       <c r="L3" s="2">
-        <f t="shared" ref="L3:L16" si="0">G3*M3</f>
+        <f t="shared" ref="L3:L16" si="0">G3*N3</f>
         <v>1360000</v>
       </c>
-      <c r="M3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="M3" s="12">
+        <f t="shared" ref="M3:M24" si="1">L3/(17900000)</f>
+        <v>7.5977653631284919E-2</v>
+      </c>
+      <c r="N3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1188,18 +1206,22 @@
         <v>14</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" ref="K4:K16" si="1">F4*M4</f>
+        <f t="shared" ref="K4:K16" si="2">F4*N4</f>
         <v>2208000</v>
       </c>
       <c r="L4" s="2">
         <f t="shared" si="0"/>
         <v>2480000</v>
       </c>
-      <c r="M4">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="M4" s="12">
+        <f t="shared" si="1"/>
+        <v>0.13854748603351955</v>
+      </c>
+      <c r="N4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1231,18 +1253,22 @@
         <v>14</v>
       </c>
       <c r="K5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2528000</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" si="0"/>
         <v>3136000</v>
       </c>
-      <c r="M5">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="M5" s="12">
+        <f t="shared" si="1"/>
+        <v>0.17519553072625699</v>
+      </c>
+      <c r="N5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1274,18 +1300,22 @@
         <v>14</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2688000</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" si="0"/>
         <v>2880000</v>
       </c>
-      <c r="M6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="M6" s="12">
+        <f t="shared" si="1"/>
+        <v>0.16089385474860335</v>
+      </c>
+      <c r="N6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1317,18 +1347,22 @@
         <v>14</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2752000</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" si="0"/>
         <v>2720000</v>
       </c>
-      <c r="M7">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="M7" s="12">
+        <f t="shared" si="1"/>
+        <v>0.15195530726256984</v>
+      </c>
+      <c r="N7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1360,18 +1394,22 @@
         <v>14</v>
       </c>
       <c r="K8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2960000</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" si="0"/>
         <v>3360000</v>
       </c>
-      <c r="M8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="M8" s="12">
+        <f t="shared" si="1"/>
+        <v>0.18770949720670391</v>
+      </c>
+      <c r="N8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1403,18 +1441,22 @@
         <v>14</v>
       </c>
       <c r="K9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2960000</v>
       </c>
       <c r="L9" s="2">
         <f t="shared" si="0"/>
         <v>2880000</v>
       </c>
-      <c r="M9">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="M9" s="12">
+        <f t="shared" si="1"/>
+        <v>0.16089385474860335</v>
+      </c>
+      <c r="N9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1446,18 +1488,22 @@
         <v>14</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3264000</v>
       </c>
       <c r="L10" s="2">
         <f t="shared" si="0"/>
         <v>3200000</v>
       </c>
-      <c r="M10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="M10" s="12">
+        <f t="shared" si="1"/>
+        <v>0.1787709497206704</v>
+      </c>
+      <c r="N10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1489,18 +1535,22 @@
         <v>14</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3024000</v>
       </c>
       <c r="L11" s="2">
         <f t="shared" si="0"/>
         <v>2960000</v>
       </c>
-      <c r="M11">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="M11" s="12">
+        <f t="shared" si="1"/>
+        <v>0.1653631284916201</v>
+      </c>
+      <c r="N11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1532,18 +1582,22 @@
         <v>13</v>
       </c>
       <c r="K12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1216000</v>
       </c>
       <c r="L12" s="2">
         <f t="shared" si="0"/>
         <v>1360000</v>
       </c>
-      <c r="M12">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="M12" s="12">
+        <f t="shared" si="1"/>
+        <v>7.5977653631284919E-2</v>
+      </c>
+      <c r="N12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1575,18 +1629,22 @@
         <v>13</v>
       </c>
       <c r="K13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>784000</v>
       </c>
       <c r="L13" s="2">
         <f t="shared" si="0"/>
         <v>864000</v>
       </c>
-      <c r="M13">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="M13" s="12">
+        <f t="shared" si="1"/>
+        <v>4.8268156424581009E-2</v>
+      </c>
+      <c r="N13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1618,18 +1676,22 @@
         <v>13</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>696000</v>
       </c>
       <c r="L14" s="2">
         <f t="shared" si="0"/>
         <v>1280000</v>
       </c>
-      <c r="M14">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="M14" s="12">
+        <f t="shared" si="1"/>
+        <v>7.150837988826815E-2</v>
+      </c>
+      <c r="N14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1661,18 +1723,22 @@
         <v>13</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>603200</v>
       </c>
       <c r="L15" s="2">
         <f t="shared" si="0"/>
         <v>720000</v>
       </c>
-      <c r="M15">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="M15" s="12">
+        <f t="shared" si="1"/>
+        <v>4.0223463687150837E-2</v>
+      </c>
+      <c r="N15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1704,18 +1770,22 @@
         <v>13</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>841600</v>
       </c>
       <c r="L16" s="2">
         <f t="shared" si="0"/>
         <v>1040000</v>
       </c>
-      <c r="M16">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="M16" s="12">
+        <f t="shared" si="1"/>
+        <v>5.8100558659217878E-2</v>
+      </c>
+      <c r="N16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1747,18 +1817,22 @@
         <v>13</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" ref="K17:K19" si="2">F17*M17</f>
+        <f t="shared" ref="K17:K19" si="3">F17*N17</f>
         <v>2704000</v>
       </c>
       <c r="L17" s="2">
-        <f t="shared" ref="L17:L19" si="3">G17*M17</f>
+        <f t="shared" ref="L17:L19" si="4">G17*N17</f>
         <v>2720000</v>
       </c>
-      <c r="M17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="M17" s="12">
+        <f t="shared" si="1"/>
+        <v>0.15195530726256984</v>
+      </c>
+      <c r="N17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1790,18 +1864,22 @@
         <v>13</v>
       </c>
       <c r="K18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>432000</v>
       </c>
       <c r="L18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>560000</v>
       </c>
-      <c r="M18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="M18" s="12">
+        <f t="shared" si="1"/>
+        <v>3.128491620111732E-2</v>
+      </c>
+      <c r="N18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1833,18 +1911,22 @@
         <v>13</v>
       </c>
       <c r="K19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>159488</v>
       </c>
       <c r="L19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>272000</v>
       </c>
-      <c r="M19">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="M19" s="12">
+        <f t="shared" si="1"/>
+        <v>1.5195530726256984E-2</v>
+      </c>
+      <c r="N19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1876,18 +1958,22 @@
         <v>13</v>
       </c>
       <c r="K20" s="2">
-        <f t="shared" ref="K20:K26" si="4">F20*M20</f>
+        <f t="shared" ref="K20:K22" si="5">F20*N20</f>
         <v>49760</v>
       </c>
       <c r="L20" s="2">
-        <f t="shared" ref="L20:L26" si="5">G20*M20</f>
+        <f t="shared" ref="L20:L22" si="6">G20*N20</f>
         <v>272000</v>
       </c>
-      <c r="M20">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="M20" s="12">
+        <f t="shared" si="1"/>
+        <v>1.5195530726256984E-2</v>
+      </c>
+      <c r="N20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1919,18 +2005,22 @@
         <v>13</v>
       </c>
       <c r="K21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>163200</v>
       </c>
       <c r="L21" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>248000</v>
       </c>
-      <c r="M21">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="M21" s="12">
+        <f t="shared" si="1"/>
+        <v>1.3854748603351955E-2</v>
+      </c>
+      <c r="N21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1962,18 +2052,22 @@
         <v>13</v>
       </c>
       <c r="K22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>37440</v>
       </c>
       <c r="L22" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>480000</v>
       </c>
-      <c r="M22">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="M22" s="12">
+        <f t="shared" si="1"/>
+        <v>2.6815642458100558E-2</v>
+      </c>
+      <c r="N22">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2005,18 +2099,22 @@
         <v>13</v>
       </c>
       <c r="K23" s="2">
-        <f t="shared" ref="K23:K26" si="6">F23*M23</f>
+        <f t="shared" ref="K23:K24" si="7">F23*N23</f>
         <v>72000</v>
       </c>
       <c r="L23" s="2">
-        <f t="shared" ref="L23:L26" si="7">G23*M23</f>
+        <f t="shared" ref="L23:L24" si="8">G23*N23</f>
         <v>432000</v>
       </c>
-      <c r="M23">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="M23" s="12">
+        <f t="shared" si="1"/>
+        <v>2.4134078212290504E-2</v>
+      </c>
+      <c r="N23">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -2048,44 +2146,48 @@
         <v>13</v>
       </c>
       <c r="K24" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>120000</v>
       </c>
       <c r="L24" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>320000</v>
       </c>
-      <c r="M24">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="M24" s="12">
+        <f t="shared" si="1"/>
+        <v>1.7877094972067038E-2</v>
+      </c>
+      <c r="N24">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="C25" s="5"/>
       <c r="D25" s="1"/>
       <c r="J25" s="5"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:14">
       <c r="C26" s="5"/>
       <c r="D26" s="1"/>
       <c r="J26" s="5"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:14">
       <c r="C27" s="5"/>
       <c r="D27" s="1"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:14">
       <c r="C28" s="5"/>
       <c r="D28" s="1"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:14">
       <c r="A30" s="8" t="s">
         <v>15</v>
       </c>
@@ -2101,7 +2203,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>